<commit_message>
FIX: Se corrige puntaje y se añaden resultados
</commit_message>
<xml_diff>
--- a/main/results/Build_Order.xlsx
+++ b/main/results/Build_Order.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
   <si>
     <t>Time</t>
   </si>
@@ -37,328 +37,295 @@
     <t>Chronoboost</t>
   </si>
   <si>
-    <t>0:00:02</t>
+    <t>0:00:09</t>
   </si>
   <si>
     <t>Assimilator</t>
   </si>
   <si>
-    <t>0:00:32</t>
+    <t>0:00:20</t>
+  </si>
+  <si>
+    <t>0:01:01</t>
+  </si>
+  <si>
+    <t>Pylon</t>
+  </si>
+  <si>
+    <t>0:01:24</t>
   </si>
   <si>
     <t>Probe</t>
   </si>
   <si>
-    <t>0:00:38</t>
+    <t>0:01:41</t>
+  </si>
+  <si>
+    <t>0:01:44</t>
+  </si>
+  <si>
+    <t>0:01:50</t>
+  </si>
+  <si>
+    <t>0:02:27</t>
+  </si>
+  <si>
+    <t>0:02:29</t>
+  </si>
+  <si>
+    <t>0:02:42</t>
   </si>
   <si>
     <t>Nexus</t>
   </si>
   <si>
-    <t>0:01:02</t>
-  </si>
-  <si>
-    <t>Pylon</t>
-  </si>
-  <si>
-    <t>0:01:14</t>
-  </si>
-  <si>
-    <t>0:01:22</t>
-  </si>
-  <si>
-    <t>0:01:26</t>
-  </si>
-  <si>
-    <t>0:01:28</t>
+    <t>0:02:45</t>
+  </si>
+  <si>
+    <t>0:02:49</t>
   </si>
   <si>
     <t>Gateway</t>
   </si>
   <si>
-    <t>0:01:32</t>
-  </si>
-  <si>
-    <t>0:01:39</t>
-  </si>
-  <si>
-    <t>0:01:58</t>
-  </si>
-  <si>
-    <t>0:02:10</t>
-  </si>
-  <si>
-    <t>0:02:25</t>
-  </si>
-  <si>
-    <t>0:02:30</t>
-  </si>
-  <si>
-    <t>0:02:40</t>
+    <t>0:02:53</t>
+  </si>
+  <si>
+    <t>0:03:02</t>
+  </si>
+  <si>
+    <t>0:03:08</t>
+  </si>
+  <si>
+    <t>0:03:11</t>
+  </si>
+  <si>
+    <t>0:03:25</t>
+  </si>
+  <si>
+    <t>Forge</t>
+  </si>
+  <si>
+    <t>0:04:01</t>
   </si>
   <si>
     <t>Cibernetics Core</t>
   </si>
   <si>
-    <t>0:02:44</t>
-  </si>
-  <si>
-    <t>0:03:02</t>
-  </si>
-  <si>
-    <t>Forge</t>
-  </si>
-  <si>
-    <t>0:03:09</t>
-  </si>
-  <si>
-    <t>0:03:23</t>
-  </si>
-  <si>
-    <t>0:03:28</t>
-  </si>
-  <si>
-    <t>0:03:31</t>
-  </si>
-  <si>
-    <t>0:03:34</t>
-  </si>
-  <si>
-    <t>0:03:36</t>
+    <t>0:04:05</t>
+  </si>
+  <si>
+    <t>0:04:21</t>
+  </si>
+  <si>
+    <t>0:04:23</t>
+  </si>
+  <si>
+    <t>0:04:37</t>
+  </si>
+  <si>
+    <t>0:04:47</t>
+  </si>
+  <si>
+    <t>Ground Weapons 1</t>
+  </si>
+  <si>
+    <t>0:04:49</t>
+  </si>
+  <si>
+    <t>0:04:54</t>
+  </si>
+  <si>
+    <t>Stalker</t>
+  </si>
+  <si>
+    <t>0:04:58</t>
+  </si>
+  <si>
+    <t>0:05:02</t>
+  </si>
+  <si>
+    <t>0:05:06</t>
+  </si>
+  <si>
+    <t>0:05:15</t>
+  </si>
+  <si>
+    <t>Shield Upgrades 1</t>
+  </si>
+  <si>
+    <t>0:05:18</t>
+  </si>
+  <si>
+    <t>Photon Cannon</t>
+  </si>
+  <si>
+    <t>0:05:20</t>
+  </si>
+  <si>
+    <t>Adept</t>
+  </si>
+  <si>
+    <t>0:05:24</t>
+  </si>
+  <si>
+    <t>Stargate</t>
+  </si>
+  <si>
+    <t>0:05:35</t>
+  </si>
+  <si>
+    <t>Warp Gate</t>
+  </si>
+  <si>
+    <t>0:05:44</t>
+  </si>
+  <si>
+    <t>Zealot</t>
+  </si>
+  <si>
+    <t>0:05:46</t>
+  </si>
+  <si>
+    <t>Air Weapons 1</t>
+  </si>
+  <si>
+    <t>0:05:54</t>
+  </si>
+  <si>
+    <t>Air Armor 1</t>
+  </si>
+  <si>
+    <t>0:05:58</t>
+  </si>
+  <si>
+    <t>0:06:00</t>
+  </si>
+  <si>
+    <t>0:06:04</t>
   </si>
   <si>
     <t>Shield Battery</t>
   </si>
   <si>
-    <t>0:03:41</t>
-  </si>
-  <si>
-    <t>Warp Gate</t>
-  </si>
-  <si>
-    <t>0:03:51</t>
-  </si>
-  <si>
-    <t>Stargate</t>
-  </si>
-  <si>
-    <t>0:03:58</t>
-  </si>
-  <si>
-    <t>0:04:00</t>
-  </si>
-  <si>
-    <t>Zealot</t>
-  </si>
-  <si>
-    <t>0:04:02</t>
-  </si>
-  <si>
-    <t>Photon Cannon</t>
-  </si>
-  <si>
-    <t>0:04:08</t>
-  </si>
-  <si>
-    <t>0:04:21</t>
-  </si>
-  <si>
-    <t>0:04:24</t>
+    <t>0:06:14</t>
+  </si>
+  <si>
+    <t>0:06:20</t>
+  </si>
+  <si>
+    <t>0:06:29</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>0:06:33</t>
+  </si>
+  <si>
+    <t>0:06:43</t>
+  </si>
+  <si>
+    <t>0:06:47</t>
+  </si>
+  <si>
+    <t>0:07:01</t>
+  </si>
+  <si>
+    <t>0:07:05</t>
+  </si>
+  <si>
+    <t>Ground Armor 1</t>
+  </si>
+  <si>
+    <t>0:07:12</t>
+  </si>
+  <si>
+    <t>Void Ray</t>
+  </si>
+  <si>
+    <t>0:07:19</t>
+  </si>
+  <si>
+    <t>0:07:22</t>
+  </si>
+  <si>
+    <t>0:07:25</t>
+  </si>
+  <si>
+    <t>0:07:27</t>
+  </si>
+  <si>
+    <t>0:07:29</t>
+  </si>
+  <si>
+    <t>0:07:32</t>
+  </si>
+  <si>
+    <t>0:07:37</t>
   </si>
   <si>
     <t>Sentry</t>
   </si>
   <si>
-    <t>0:04:27</t>
-  </si>
-  <si>
-    <t>0:04:30</t>
-  </si>
-  <si>
-    <t>0:04:36</t>
-  </si>
-  <si>
-    <t>Air Armor 1</t>
-  </si>
-  <si>
-    <t>0:04:39</t>
-  </si>
-  <si>
-    <t>0:04:41</t>
-  </si>
-  <si>
-    <t>0:04:48</t>
-  </si>
-  <si>
-    <t>0:04:54</t>
-  </si>
-  <si>
-    <t>0:05:02</t>
-  </si>
-  <si>
-    <t>Stalker</t>
-  </si>
-  <si>
-    <t>0:05:04</t>
-  </si>
-  <si>
-    <t>0:05:08</t>
-  </si>
-  <si>
-    <t>0:05:11</t>
-  </si>
-  <si>
-    <t>0:05:16</t>
-  </si>
-  <si>
-    <t>0:05:18</t>
-  </si>
-  <si>
-    <t>0:05:22</t>
-  </si>
-  <si>
-    <t>0:05:25</t>
-  </si>
-  <si>
-    <t>Air Weapons 1</t>
-  </si>
-  <si>
-    <t>0:05:28</t>
-  </si>
-  <si>
-    <t>Void Ray</t>
-  </si>
-  <si>
-    <t>0:05:30</t>
-  </si>
-  <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
-    <t>0:05:32</t>
-  </si>
-  <si>
-    <t>0:05:34</t>
-  </si>
-  <si>
-    <t>Ground Armor 1</t>
-  </si>
-  <si>
-    <t>0:05:38</t>
-  </si>
-  <si>
-    <t>0:05:42</t>
-  </si>
-  <si>
-    <t>0:05:57</t>
-  </si>
-  <si>
-    <t>Adept</t>
-  </si>
-  <si>
-    <t>0:06:01</t>
-  </si>
-  <si>
-    <t>0:06:03</t>
-  </si>
-  <si>
-    <t>0:06:08</t>
-  </si>
-  <si>
-    <t>0:06:11</t>
-  </si>
-  <si>
-    <t>0:06:15</t>
-  </si>
-  <si>
-    <t>0:06:22</t>
-  </si>
-  <si>
-    <t>0:06:25</t>
-  </si>
-  <si>
-    <t>0:06:27</t>
-  </si>
-  <si>
-    <t>Fleet Beacon</t>
-  </si>
-  <si>
-    <t>0:06:32</t>
-  </si>
-  <si>
-    <t>0:06:35</t>
-  </si>
-  <si>
-    <t>0:06:46</t>
-  </si>
-  <si>
-    <t>0:06:49</t>
-  </si>
-  <si>
-    <t>Shield Upgrades 1</t>
-  </si>
-  <si>
-    <t>0:06:51</t>
-  </si>
-  <si>
-    <t>0:07:00</t>
-  </si>
-  <si>
-    <t>0:07:07</t>
-  </si>
-  <si>
-    <t>0:07:16</t>
-  </si>
-  <si>
-    <t>0:07:18</t>
-  </si>
-  <si>
-    <t>0:07:21</t>
-  </si>
-  <si>
-    <t>0:07:23</t>
-  </si>
-  <si>
-    <t>0:07:33</t>
-  </si>
-  <si>
-    <t>Air Weapons 2</t>
-  </si>
-  <si>
-    <t>0:07:36</t>
-  </si>
-  <si>
-    <t>0:07:38</t>
-  </si>
-  <si>
-    <t>Flux Vanes</t>
-  </si>
-  <si>
-    <t>0:07:40</t>
-  </si>
-  <si>
     <t>0:07:42</t>
   </si>
   <si>
+    <t>0:07:46</t>
+  </si>
+  <si>
     <t>0:07:49</t>
   </si>
   <si>
-    <t>0:07:56</t>
+    <t>0:07:52</t>
   </si>
   <si>
     <t>0:08:01</t>
   </si>
   <si>
-    <t>0:08:05</t>
-  </si>
-  <si>
-    <t>Robotics Facility</t>
-  </si>
-  <si>
-    <t>0:08:12</t>
+    <t>0:08:08</t>
+  </si>
+  <si>
+    <t>0:08:30</t>
+  </si>
+  <si>
+    <t>0:08:34</t>
+  </si>
+  <si>
+    <t>0:08:44</t>
+  </si>
+  <si>
+    <t>0:08:46</t>
+  </si>
+  <si>
+    <t>0:08:53</t>
+  </si>
+  <si>
+    <t>0:08:56</t>
   </si>
   <si>
     <t>Twilight Council</t>
+  </si>
+  <si>
+    <t>0:09:09</t>
+  </si>
+  <si>
+    <t>0:09:11</t>
+  </si>
+  <si>
+    <t>0:09:14</t>
+  </si>
+  <si>
+    <t>0:09:21</t>
+  </si>
+  <si>
+    <t>0:09:30</t>
+  </si>
+  <si>
+    <t>0:09:34</t>
+  </si>
+  <si>
+    <t>0:09:40</t>
   </si>
 </sst>
 </file>
@@ -690,7 +657,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -733,7 +700,7 @@
         <v>15</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>94</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -744,7 +711,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>13</v>
@@ -753,21 +720,18 @@
         <v>15</v>
       </c>
       <c r="E3">
-        <v>367</v>
+        <v>138</v>
       </c>
       <c r="F3">
-        <v>36</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4">
         <v>13</v>
@@ -776,78 +740,84 @@
         <v>15</v>
       </c>
       <c r="E4">
-        <v>26</v>
+        <v>514</v>
       </c>
       <c r="F4">
-        <v>56</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
       <c r="C5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>218</v>
+        <v>776</v>
       </c>
       <c r="F5">
-        <v>148</v>
+        <v>324</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>14</v>
       </c>
       <c r="D6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E6">
-        <v>260</v>
+        <v>899</v>
       </c>
       <c r="F6">
-        <v>192</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>14</v>
       </c>
       <c r="D7">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E7">
-        <v>249</v>
+        <v>924</v>
       </c>
       <c r="F7">
-        <v>220</v>
+        <v>450</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>14</v>
@@ -856,110 +826,113 @@
         <v>20</v>
       </c>
       <c r="E8">
-        <v>188</v>
+        <v>889</v>
       </c>
       <c r="F8">
-        <v>232</v>
+        <v>485</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E9">
-        <v>51</v>
+        <v>1280</v>
       </c>
       <c r="F9">
-        <v>236</v>
+        <v>803</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E10">
-        <v>14</v>
+        <v>1294</v>
       </c>
       <c r="F10">
-        <v>248</v>
+        <v>813</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>25</v>
       </c>
       <c r="E11">
-        <v>16</v>
+        <v>1063</v>
       </c>
       <c r="F11">
-        <v>272</v>
+        <v>933</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D12">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E12">
-        <v>159</v>
+        <v>692</v>
       </c>
       <c r="F12">
-        <v>360</v>
+        <v>953</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
       <c r="C13">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D13">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E13">
-        <v>150</v>
+        <v>586</v>
       </c>
       <c r="F13">
-        <v>461</v>
+        <v>983</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -967,19 +940,19 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D14">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E14">
-        <v>180</v>
+        <v>530</v>
       </c>
       <c r="F14">
-        <v>601</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -987,22 +960,19 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E15">
-        <v>231</v>
+        <v>497</v>
       </c>
       <c r="F15">
-        <v>641</v>
-      </c>
-      <c r="G15" t="s">
-        <v>6</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1010,85 +980,79 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E16">
-        <v>197</v>
+        <v>471</v>
       </c>
       <c r="F16">
-        <v>731</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="E17">
-        <v>239</v>
+        <v>114</v>
       </c>
       <c r="F17">
-        <v>761</v>
-      </c>
-      <c r="G17" t="s">
-        <v>6</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
         <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
       </c>
       <c r="C18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="E18">
-        <v>330</v>
+        <v>155</v>
       </c>
       <c r="F18">
-        <v>931</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
       </c>
       <c r="C19">
         <v>16</v>
       </c>
       <c r="D19">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E19">
-        <v>418</v>
+        <v>518</v>
       </c>
       <c r="F19">
-        <v>991</v>
-      </c>
-      <c r="G19" t="s">
-        <v>6</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1096,19 +1060,19 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E20">
-        <v>613</v>
+        <v>562</v>
       </c>
       <c r="F20">
-        <v>1121</v>
+        <v>1683</v>
       </c>
       <c r="G20" t="s">
         <v>6</v>
@@ -1119,19 +1083,19 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>17</v>
       </c>
       <c r="D21">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E21">
-        <v>601</v>
+        <v>638</v>
       </c>
       <c r="F21">
-        <v>1161</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1139,19 +1103,19 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>17</v>
       </c>
       <c r="D22">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E22">
-        <v>232</v>
+        <v>579</v>
       </c>
       <c r="F22">
-        <v>1181</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1159,19 +1123,19 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>17</v>
       </c>
       <c r="D23">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E23">
-        <v>113</v>
+        <v>706</v>
       </c>
       <c r="F23">
-        <v>1201</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1182,16 +1146,19 @@
         <v>37</v>
       </c>
       <c r="C24">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E24">
-        <v>30</v>
+        <v>846</v>
       </c>
       <c r="F24">
-        <v>1211</v>
+        <v>2066</v>
+      </c>
+      <c r="G24" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1199,162 +1166,168 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C25">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E25">
-        <v>95</v>
+        <v>462</v>
       </c>
       <c r="F25">
-        <v>1251</v>
-      </c>
-      <c r="G25" t="s">
-        <v>6</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
         <v>40</v>
       </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
       <c r="C26">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E26">
-        <v>94</v>
+        <v>524</v>
       </c>
       <c r="F26">
-        <v>1191</v>
+        <v>2131</v>
+      </c>
+      <c r="G26" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C27">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E27">
-        <v>118</v>
+        <v>571</v>
       </c>
       <c r="F27">
-        <v>1257</v>
+        <v>2170</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C28">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D28">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E28">
-        <v>134</v>
+        <v>218</v>
       </c>
       <c r="F28">
-        <v>1270</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C29">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D29">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>114</v>
       </c>
       <c r="F29">
-        <v>1283</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C30">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D30">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E30">
-        <v>8</v>
+        <v>239</v>
       </c>
       <c r="F30">
-        <v>1348</v>
+        <v>2376</v>
+      </c>
+      <c r="G30" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C31">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D31">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E31">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F31">
-        <v>1517</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
         <v>49</v>
       </c>
-      <c r="B32" t="s">
-        <v>50</v>
-      </c>
       <c r="C32">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D32">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E32">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="F32">
-        <v>1546</v>
+        <v>2424</v>
       </c>
       <c r="G32" t="s">
         <v>6</v>
@@ -1362,22 +1335,22 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="s">
         <v>51</v>
       </c>
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
       <c r="C33">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D33">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E33">
-        <v>188</v>
+        <v>32</v>
       </c>
       <c r="F33">
-        <v>1578</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1385,488 +1358,509 @@
         <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="C34">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D34">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E34">
-        <v>71</v>
+        <v>188</v>
       </c>
       <c r="F34">
-        <v>1610</v>
+        <v>2482</v>
+      </c>
+      <c r="G34" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C35">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D35">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E35">
-        <v>153</v>
+        <v>313</v>
       </c>
       <c r="F35">
-        <v>1696</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C36">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D36">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E36">
-        <v>36</v>
+        <v>328</v>
       </c>
       <c r="F36">
-        <v>1732</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="C37">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D37">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E37">
-        <v>53</v>
+        <v>437</v>
       </c>
       <c r="F37">
-        <v>1750</v>
+        <v>2738</v>
+      </c>
+      <c r="G37" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C38">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D38">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E38">
-        <v>52</v>
+        <v>484</v>
       </c>
       <c r="F38">
-        <v>1858</v>
+        <v>2786</v>
+      </c>
+      <c r="G38" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C39">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D39">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E39">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="F39">
-        <v>1951</v>
+        <v>2802</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C40">
         <v>25</v>
       </c>
       <c r="D40">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="E40">
-        <v>159</v>
+        <v>46</v>
       </c>
       <c r="F40">
-        <v>2084</v>
-      </c>
-      <c r="G40" t="s">
-        <v>6</v>
+        <v>2850</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C41">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D41">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="E41">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="F41">
-        <v>2122</v>
-      </c>
-      <c r="G41" t="s">
-        <v>6</v>
+        <v>2994</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C42">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D42">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E42">
-        <v>96</v>
+        <v>264</v>
       </c>
       <c r="F42">
-        <v>2179</v>
+        <v>3074</v>
+      </c>
+      <c r="G42" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C43">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D43">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E43">
-        <v>30</v>
+        <v>389</v>
       </c>
       <c r="F43">
-        <v>2217</v>
+        <v>3202</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C44">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D44">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E44">
-        <v>100</v>
+        <v>436</v>
       </c>
       <c r="F44">
-        <v>2293</v>
+        <v>3250</v>
+      </c>
+      <c r="G44" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C45">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D45">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E45">
-        <v>117</v>
+        <v>576</v>
       </c>
       <c r="F45">
-        <v>2312</v>
+        <v>3394</v>
+      </c>
+      <c r="G45" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C46">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D46">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E46">
-        <v>170</v>
+        <v>472</v>
       </c>
       <c r="F46">
-        <v>2369</v>
+        <v>3442</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" t="s">
         <v>67</v>
       </c>
-      <c r="B47" t="s">
-        <v>68</v>
-      </c>
       <c r="C47">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D47">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E47">
-        <v>204</v>
+        <v>675</v>
       </c>
       <c r="F47">
-        <v>2407</v>
+        <v>3650</v>
+      </c>
+      <c r="G47" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C48">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D48">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E48">
-        <v>239</v>
+        <v>722</v>
       </c>
       <c r="F48">
-        <v>2445</v>
+        <v>3698</v>
+      </c>
+      <c r="G48" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C49">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D49">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E49">
-        <v>257</v>
+        <v>815</v>
       </c>
       <c r="F49">
-        <v>2464</v>
+        <v>3794</v>
+      </c>
+      <c r="G49" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C50">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D50">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E50">
-        <v>276</v>
+        <v>758</v>
       </c>
       <c r="F50">
-        <v>2483</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="C51">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D51">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E51">
-        <v>294</v>
+        <v>640</v>
       </c>
       <c r="F51">
-        <v>2502</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C52">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D52">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E52">
-        <v>199</v>
+        <v>521</v>
       </c>
       <c r="F52">
-        <v>2559</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C53">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D53">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="E53">
-        <v>104</v>
+        <v>536</v>
       </c>
       <c r="F53">
-        <v>2466</v>
+        <v>3970</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D54">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E54">
-        <v>361</v>
+        <v>152</v>
       </c>
       <c r="F54">
-        <v>2732</v>
-      </c>
-      <c r="G54" t="s">
-        <v>6</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55">
         <v>37</v>
       </c>
-      <c r="C55">
-        <v>36</v>
-      </c>
       <c r="D55">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E55">
-        <v>315</v>
+        <v>33</v>
       </c>
       <c r="F55">
-        <v>2789</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="C56">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D56">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E56">
-        <v>334</v>
+        <v>110</v>
       </c>
       <c r="F56">
-        <v>2808</v>
+        <v>4098</v>
+      </c>
+      <c r="G56" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C57">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D57">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E57">
-        <v>407</v>
+        <v>173</v>
       </c>
       <c r="F57">
-        <v>2884</v>
+        <v>4162</v>
       </c>
       <c r="G57" t="s">
         <v>6</v>
@@ -1874,185 +1868,185 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C58">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D58">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E58">
-        <v>444</v>
+        <v>219</v>
       </c>
       <c r="F58">
-        <v>2922</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C59">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D59">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E59">
-        <v>349</v>
+        <v>151</v>
       </c>
       <c r="F59">
-        <v>2979</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C60">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D60">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E60">
-        <v>309</v>
+        <v>32</v>
       </c>
       <c r="F60">
-        <v>3093</v>
+        <v>4124</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C61">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D61">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E61">
-        <v>345</v>
+        <v>6</v>
       </c>
       <c r="F61">
-        <v>3131</v>
-      </c>
-      <c r="G61" t="s">
-        <v>6</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="C62">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D62">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E62">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>2950</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="C63">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D63">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="E63">
-        <v>137</v>
+        <v>252</v>
       </c>
       <c r="F63">
-        <v>3026</v>
+        <v>4684</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="C64">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D64">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="E64">
-        <v>23</v>
+        <v>298</v>
       </c>
       <c r="F64">
-        <v>3064</v>
+        <v>4732</v>
+      </c>
+      <c r="G64" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C65">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D65">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="E65">
-        <v>207</v>
+        <v>339</v>
       </c>
       <c r="F65">
-        <v>3254</v>
+        <v>4876</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="C66">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D66">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="E66">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="F66">
-        <v>3292</v>
+        <v>4892</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2060,19 +2054,22 @@
         <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C67">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D67">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="E67">
-        <v>262</v>
+        <v>298</v>
       </c>
       <c r="F67">
-        <v>3311</v>
+        <v>4988</v>
+      </c>
+      <c r="G67" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2080,59 +2077,62 @@
         <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C68">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D68">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="E68">
-        <v>108</v>
+        <v>179</v>
       </c>
       <c r="F68">
-        <v>3263</v>
+        <v>4920</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="C69">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D69">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="E69">
-        <v>68</v>
+        <v>366</v>
       </c>
       <c r="F69">
-        <v>3377</v>
+        <v>5121</v>
+      </c>
+      <c r="G69" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C70">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D70">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="E70">
-        <v>215</v>
+        <v>381</v>
       </c>
       <c r="F70">
-        <v>3529</v>
+        <v>5138</v>
       </c>
       <c r="G70" t="s">
         <v>6</v>
@@ -2140,82 +2140,85 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C71">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D71">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="E71">
-        <v>233</v>
+        <v>412</v>
       </c>
       <c r="F71">
-        <v>3548</v>
+        <v>5172</v>
+      </c>
+      <c r="G71" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="C72">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D72">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="E72">
-        <v>270</v>
+        <v>356</v>
       </c>
       <c r="F72">
-        <v>3586</v>
+        <v>5174</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C73">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D73">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="E73">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="F73">
-        <v>3605</v>
+        <v>5310</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C74">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D74">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="E74">
-        <v>378</v>
+        <v>127</v>
       </c>
       <c r="F74">
-        <v>3776</v>
+        <v>5361</v>
       </c>
       <c r="G74" t="s">
         <v>6</v>
@@ -2226,182 +2229,19 @@
         <v>103</v>
       </c>
       <c r="B75" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C75">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D75">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="E75">
-        <v>414</v>
+        <v>55</v>
       </c>
       <c r="F75">
-        <v>3814</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>104</v>
-      </c>
-      <c r="B76" t="s">
-        <v>105</v>
-      </c>
-      <c r="C76">
-        <v>60</v>
-      </c>
-      <c r="D76">
-        <v>75</v>
-      </c>
-      <c r="E76">
-        <v>433</v>
-      </c>
-      <c r="F76">
-        <v>3833</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>106</v>
-      </c>
-      <c r="B77" t="s">
-        <v>19</v>
-      </c>
-      <c r="C77">
-        <v>60</v>
-      </c>
-      <c r="D77">
-        <v>75</v>
-      </c>
-      <c r="E77">
-        <v>301</v>
-      </c>
-      <c r="F77">
-        <v>3852</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" t="s">
-        <v>107</v>
-      </c>
-      <c r="B78" t="s">
-        <v>88</v>
-      </c>
-      <c r="C78">
-        <v>60</v>
-      </c>
-      <c r="D78">
-        <v>75</v>
-      </c>
-      <c r="E78">
-        <v>19</v>
-      </c>
-      <c r="F78">
-        <v>3671</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" t="s">
-        <v>108</v>
-      </c>
-      <c r="B79" t="s">
-        <v>37</v>
-      </c>
-      <c r="C79">
-        <v>60</v>
-      </c>
-      <c r="D79">
-        <v>75</v>
-      </c>
-      <c r="E79">
-        <v>29</v>
-      </c>
-      <c r="F79">
-        <v>3785</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" t="s">
-        <v>109</v>
-      </c>
-      <c r="B80" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80">
-        <v>62</v>
-      </c>
-      <c r="D80">
-        <v>75</v>
-      </c>
-      <c r="E80">
-        <v>139</v>
-      </c>
-      <c r="F80">
-        <v>3904</v>
-      </c>
-      <c r="G80" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" t="s">
-        <v>110</v>
-      </c>
-      <c r="B81" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81">
-        <v>62</v>
-      </c>
-      <c r="D81">
-        <v>75</v>
-      </c>
-      <c r="E81">
-        <v>213</v>
-      </c>
-      <c r="F81">
-        <v>3984</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" t="s">
-        <v>111</v>
-      </c>
-      <c r="B82" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82">
-        <v>62</v>
-      </c>
-      <c r="D82">
-        <v>75</v>
-      </c>
-      <c r="E82">
-        <v>118</v>
-      </c>
-      <c r="F82">
-        <v>3944</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" t="s">
-        <v>113</v>
-      </c>
-      <c r="B83" t="s">
-        <v>114</v>
-      </c>
-      <c r="C83">
-        <v>66</v>
-      </c>
-      <c r="D83">
-        <v>75</v>
-      </c>
-      <c r="E83">
-        <v>83</v>
-      </c>
-      <c r="F83">
-        <v>3970</v>
+        <v>5446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>